<commit_message>
Added a blender file, which will just be a whiteboard, and added a sheet to the excel file. All of this will contain various considerations a motor controller will need to encompass. The practicallity of this is not as a checklist per se for a good motor controller, as this is more like the bare minimums for controllers, but rather a way for me to actually understand the equipment that we are going to end up using
</commit_message>
<xml_diff>
--- a/Potential supplies/Potential options excel.xlsx
+++ b/Potential supplies/Potential options excel.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ronitbhandari/Desktop/VELOX/Potential supplies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E3CC76B-9DF4-C740-9375-218A02B3EC0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{229ED164-F644-6C41-8775-5473B2E5B7EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{E61430C9-24AE-4345-A119-839ABEBDFB5D}"/>
+    <workbookView xWindow="4440" yWindow="740" windowWidth="24960" windowHeight="18380" activeTab="1" xr2:uid="{E61430C9-24AE-4345-A119-839ABEBDFB5D}"/>
   </bookViews>
   <sheets>
     <sheet name="Motor Controllers" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,8 +36,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLRICHVALUE" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <valueMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </valueMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t>MOTOR CONTROLLERS</t>
   </si>
@@ -128,6 +151,31 @@
   </si>
   <si>
     <t>Nominal Power Rating (kW)</t>
+  </si>
+  <si>
+    <t>General problems with motors
+(In general are all adressed by motor controllers)</t>
+  </si>
+  <si>
+    <t>Problem</t>
+  </si>
+  <si>
+    <t>Solution</t>
+  </si>
+  <si>
+    <t>Flyback Diode</t>
+  </si>
+  <si>
+    <t>Add a reverse diode parallel to the motor
+(Schotty Diodes are normally used)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">High voltage spike occurs on shutdown
+A massive amount of voltage is pushed 
+backwards, in reverse, through the motor </t>
+  </si>
+  <si>
+    <t>Image</t>
   </si>
 </sst>
 </file>
@@ -237,40 +285,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -279,11 +330,7 @@
   </cellStyles>
   <dxfs count="12">
     <dxf>
-      <font>
-        <b/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -295,13 +342,14 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -345,6 +393,9 @@
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -358,23 +409,87 @@
 </styleSheet>
 </file>
 
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_ClassificationId">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <rv s="0">
+    <v>0</v>
+    <v>5</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <s t="_localImage">
+    <k n="_rvRel:LocalImageIdentifier" t="i"/>
+    <k n="CalcOrigin" t="i"/>
+  </s>
+</rvStructures>
+</file>
+
+<file path=xl/richData/richValueRel.xml><?xml version="1.0" encoding="utf-8"?>
+<richValueRels xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/richvaluerel" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rel r:id="rId1"/>
+</richValueRels>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1A55E5A3-C972-7B4E-B9B6-9EDBED53392B}" name="Table1" displayName="Table1" ref="B3:L5" totalsRowShown="0" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1A55E5A3-C972-7B4E-B9B6-9EDBED53392B}" name="Table1" displayName="Table1" ref="B3:L5" totalsRowShown="0" dataDxfId="11">
   <autoFilter ref="B3:L5" xr:uid="{1A55E5A3-C972-7B4E-B9B6-9EDBED53392B}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{6C021C61-FE4E-4048-9442-3BB53D8C716F}" name="Link" dataDxfId="11" dataCellStyle="Hyperlink"/>
-    <tableColumn id="10" xr3:uid="{02796E71-1095-4840-BAD9-FD7B6F39CAA0}" name="Outlet" dataDxfId="10" dataCellStyle="Hyperlink"/>
-    <tableColumn id="2" xr3:uid="{93C36F7A-A6B8-944F-BCCF-AD936FAEC481}" name="NAME" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{3FA2BACB-C519-C14E-A117-12D24A0E085E}" name="Price" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{83107570-CAF6-5A4D-8EFE-0119794E56C3}" name="Voltage M+" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{CECE7CD4-D045-374F-B7BB-B91654B35EA5}" name="Voltage m-" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{325D58FA-3D05-0544-AD80-F4908D2218BB}" name="Coasting Current M+" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{98138A37-9981-E94A-A2F5-26C2C67D4419}" name="Peak Current M+" dataDxfId="2"/>
-    <tableColumn id="11" xr3:uid="{B82DBA90-3471-D647-B73A-1786C3958F06}" name="Nominal Power Rating (kW)" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{6C021C61-FE4E-4048-9442-3BB53D8C716F}" name="Link" dataDxfId="10" dataCellStyle="Hyperlink"/>
+    <tableColumn id="10" xr3:uid="{02796E71-1095-4840-BAD9-FD7B6F39CAA0}" name="Outlet" dataDxfId="9" dataCellStyle="Hyperlink"/>
+    <tableColumn id="2" xr3:uid="{93C36F7A-A6B8-944F-BCCF-AD936FAEC481}" name="NAME" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{3FA2BACB-C519-C14E-A117-12D24A0E085E}" name="Price" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{83107570-CAF6-5A4D-8EFE-0119794E56C3}" name="Voltage M+" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{CECE7CD4-D045-374F-B7BB-B91654B35EA5}" name="Voltage m-" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{325D58FA-3D05-0544-AD80-F4908D2218BB}" name="Coasting Current M+" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{98138A37-9981-E94A-A2F5-26C2C67D4419}" name="Peak Current M+" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{B82DBA90-3471-D647-B73A-1786C3958F06}" name="Nominal Power Rating (kW)" dataDxfId="2">
       <calculatedColumnFormula>Table1[[#This Row],[Voltage M+]]*(Table1[[#This Row],[Coasting Current M+]]*0.9)/1000</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" xr3:uid="{C188315A-AFBE-8143-AA8C-19B266EABBD0}" name="Compatible with PiPico? " dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{9BDDAFBE-B8EA-9445-AE1D-3BCF29F2FC81}" name="Notes" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{9BDDAFBE-B8EA-9445-AE1D-3BCF29F2FC81}" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -699,7 +814,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{186C5108-A6D5-724A-BD56-A7CA961CB313}">
   <dimension ref="B2:P6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
@@ -768,44 +883,44 @@
       <c r="L3" t="s">
         <v>18</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="O3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="P3" s="1"/>
+      <c r="P3" s="10"/>
     </row>
     <row r="4" spans="2:16" ht="65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>92.04</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <v>58</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="3">
         <v>7</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="3">
         <v>25</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="3">
         <v>60</v>
       </c>
-      <c r="J4" s="3">
+      <c r="J4" s="2">
         <f>Table1[[#This Row],[Voltage M+]]*(Table1[[#This Row],[Coasting Current M+]]*0.9)/1000</f>
         <v>1.3049999999999999</v>
       </c>
-      <c r="K4" s="9" t="s">
+      <c r="K4" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="L4" s="10" t="s">
+      <c r="L4" s="9" t="s">
         <v>25</v>
       </c>
       <c r="O4" t="s">
@@ -816,38 +931,38 @@
       </c>
     </row>
     <row r="5" spans="2:16" ht="64" x14ac:dyDescent="0.2">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>117</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="6">
         <v>45</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="3">
         <v>10</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="3">
         <v>40</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="3">
         <v>80</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J5" s="2">
         <f>Table1[[#This Row],[Voltage M+]]*(Table1[[#This Row],[Coasting Current M+]]*0.9)/1000</f>
         <v>1.62</v>
       </c>
-      <c r="K5" s="9" t="s">
+      <c r="K5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="L5" s="10" t="s">
+      <c r="L5" s="9" t="s">
         <v>26</v>
       </c>
       <c r="O5" t="s">
@@ -879,4 +994,55 @@
     <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4776E94B-32CC-AC47-84D9-E689900C075F}">
+  <dimension ref="A2:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="144" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="43.6640625" customWidth="1"/>
+    <col min="2" max="2" width="32.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="B2" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="148" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>